<commit_message>
finilize sound effect of star and cloud
</commit_message>
<xml_diff>
--- a/Asset Source.xlsx
+++ b/Asset Source.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8260" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="8260" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pistures" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>background1.mp3</t>
   </si>
@@ -29,17 +29,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ding</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>音效</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>www.soundrangers.com</t>
-  </si>
-  <si>
     <t>背景音乐</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -52,6 +45,16 @@
   </si>
   <si>
     <t>http://www.clipartpanda.com/clipart_images/shared-by-lucjor-1658623</t>
+  </si>
+  <si>
+    <t>sound_star</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.2gei.com/sound/class/piano/</t>
+  </si>
+  <si>
+    <t>钢琴音符85个_mp3/65!</t>
   </si>
 </sst>
 </file>
@@ -430,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -441,10 +444,10 @@
   <sheetData>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -462,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -479,23 +482,23 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>1.95</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -503,7 +506,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
draw the bubble myself ^_^
</commit_message>
<xml_diff>
--- a/Asset Source.xlsx
+++ b/Asset Source.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Pistures" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>background1.mp3</t>
   </si>
@@ -118,32 +118,47 @@
     <t>https://www.makeschool.com/academy/art/object/game-icons/cog-lock</t>
   </si>
   <si>
+    <t>CC0 Public Domain </t>
+  </si>
+  <si>
+    <t>License Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>License Link</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://pixabay.com/en/service/terms/#download_terms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC BY 3.0  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://creativecommons.org/licenses/by/3.0/</t>
+  </si>
+  <si>
+    <t>http://pixabay.com/en/bubble-circle-glossy-blue-air-151854/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Bubble</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CC0 Public Domain </t>
-  </si>
-  <si>
-    <t>License Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>License Link</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://pixabay.com/en/bubble-circle-glossy-blue-air-151854/</t>
-  </si>
-  <si>
-    <t>http://pixabay.com/en/service/terms/#download_terms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC BY 3.0  </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://creativecommons.org/licenses/by/3.0/</t>
+    <t>Bubble Blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bubble gray</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://photobucket.com/terms</t>
+  </si>
+  <si>
+    <t>http://smg.photobucket.com/user/PrayciousAnjel/media/Fantasy%20Crests/Fantasy%20Orbs/glassorb1.png.html</t>
   </si>
 </sst>
 </file>
@@ -209,7 +224,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -223,13 +238,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="22">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
@@ -239,11 +262,19 @@
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="20" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -572,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:E6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -593,10 +624,10 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
         <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
       </c>
       <c r="F1" t="s">
         <v>11</v>
@@ -655,10 +686,10 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
         <v>21</v>
@@ -675,10 +706,10 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
         <v>26</v>
@@ -686,22 +717,39 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change the ground picture
</commit_message>
<xml_diff>
--- a/Asset Source.xlsx
+++ b/Asset Source.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="16080" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Pistures" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>background1.mp3</t>
   </si>
@@ -173,6 +173,22 @@
   </si>
   <si>
     <t>File:F icon.svg</t>
+  </si>
+  <si>
+    <t>Ground</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://creativecommons.org/publicdomain/mark/1.0/</t>
+  </si>
+  <si>
+    <t>Public Domain Mark 1.0</t>
+  </si>
+  <si>
+    <t>No Copyright</t>
+  </si>
+  <si>
+    <t>https://www.makeschool.com/academy/art/object/assorted-clouds</t>
   </si>
 </sst>
 </file>
@@ -617,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -778,6 +794,23 @@
       </c>
       <c r="F11" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Bubble Pop Up assets and animation
</commit_message>
<xml_diff>
--- a/Asset Source.xlsx
+++ b/Asset Source.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="880" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Pistures" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>background1.mp3</t>
   </si>
@@ -40,13 +40,6 @@
     <t>http://www.2gei.com/music/class/light_2/</t>
   </si>
   <si>
-    <t>Play-button</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://www.clipartpanda.com/clipart_images/shared-by-lucjor-1658623</t>
-  </si>
-  <si>
     <t>sound_star</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -189,6 +182,13 @@
   </si>
   <si>
     <t>https://www.makeschool.com/academy/art/object/assorted-clouds</t>
+  </si>
+  <si>
+    <t>https://www.makeschool.com/academy/art/level-design/basic-platform-tiles</t>
+  </si>
+  <si>
+    <t>Button_Play</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -636,7 +636,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -648,169 +648,178 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
         <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
         <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
         <v>36</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="F11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" t="s">
         <v>43</v>
       </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" t="s">
         <v>45</v>
-      </c>
-      <c r="E13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -851,13 +860,13 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3">

</xml_diff>

<commit_message>
shop on main scene working
</commit_message>
<xml_diff>
--- a/Asset Source.xlsx
+++ b/Asset Source.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6020" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Pistures" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>background1.mp3</t>
   </si>
@@ -186,6 +186,13 @@
   <si>
     <t>Button_Play</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Button Shopping Cart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.flaticon.com/authors/google</t>
   </si>
 </sst>
 </file>
@@ -251,7 +258,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -265,6 +272,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -279,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="26">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
@@ -293,6 +304,8 @@
     <cellStyle name="访问过的超链接" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -302,6 +315,8 @@
     <cellStyle name="超链接" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="24" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -630,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -718,110 +733,133 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" t="s">
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F8" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" t="s">
-        <v>37</v>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
         <v>40</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C16" t="s">
         <v>43</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D16" t="s">
         <v>42</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E16" t="s">
         <v>41</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F16" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
save 5 scores locally
</commit_message>
<xml_diff>
--- a/Asset Source.xlsx
+++ b/Asset Source.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>background1.mp3</t>
   </si>
@@ -95,9 +95,6 @@
     <t>anthem</t>
   </si>
   <si>
-    <t>Attribution, Commercially, Modify</t>
-  </si>
-  <si>
     <t>Button Setting</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -193,6 +190,13 @@
   </si>
   <si>
     <t>http://www.flaticon.com/authors/google</t>
+  </si>
+  <si>
+    <t>Button trophy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.makeschool.com/academy/art/object/game-icons/trophy</t>
   </si>
 </sst>
 </file>
@@ -258,7 +262,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -272,6 +276,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -290,7 +298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="26">
+  <cellStyles count="30">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
@@ -306,6 +314,8 @@
     <cellStyle name="访问过的超链接" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -317,6 +327,8 @@
     <cellStyle name="超链接" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="28" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -645,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C8" sqref="C8:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -666,10 +678,10 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
         <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
       </c>
       <c r="F1" t="s">
         <v>9</v>
@@ -677,19 +689,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -703,10 +715,10 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
@@ -723,10 +735,10 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
@@ -745,14 +757,14 @@
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>20</v>
+      <c r="C8" t="s">
+        <v>27</v>
       </c>
       <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
         <v>28</v>
-      </c>
-      <c r="E8" t="s">
-        <v>29</v>
       </c>
       <c r="F8" t="s">
         <v>18</v>
@@ -760,107 +772,124 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
         <v>28</v>
       </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" t="s">
-        <v>30</v>
+      <c r="F11" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" t="s">
         <v>36</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
         <v>40</v>
       </c>
-      <c r="C16" t="s">
+      <c r="F17" t="s">
         <v>43</v>
-      </c>
-      <c r="D16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>